<commit_message>
changing sources for O4 and O5
</commit_message>
<xml_diff>
--- a/csdata/O/SI/O4+.xlsx
+++ b/csdata/O/SI/O4+.xlsx
@@ -28,14 +28,14 @@
     <t>Ref</t>
   </si>
   <si>
-    <t>Measured electron-impact ionization of Be-like ions: B+, C2+, N3+, and O~ Falk 1983</t>
+    <t>ELECTRON-IMPACT IONIZATION OF Be-LIKE C iii, N iv, AND O v, Fogle 2008</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -49,6 +49,11 @@
     </font>
     <font>
       <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -81,12 +86,12 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -99,7 +104,7 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="11" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
@@ -340,15 +345,15 @@
     </row>
     <row r="2">
       <c r="A2" s="3">
-        <v>104.0</v>
-      </c>
-      <c r="B2" s="4">
-        <v>0.09</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="D2" s="3">
+        <v>95.7</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.025</v>
+      </c>
+      <c r="D2" s="4">
         <v>-18.0</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -357,362 +362,494 @@
     </row>
     <row r="3">
       <c r="A3" s="3">
-        <v>109.0</v>
-      </c>
-      <c r="B3" s="4">
-        <v>0.37</v>
-      </c>
-      <c r="C3" s="4">
+        <v>100.6</v>
+      </c>
+      <c r="B3" s="3">
         <v>0.05</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.025</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" s="3">
-        <v>113.0</v>
-      </c>
-      <c r="B4" s="4">
-        <v>0.48</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.06</v>
+        <v>108.7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.015</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" s="3">
-        <v>118.0</v>
-      </c>
-      <c r="B5" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.05</v>
+        <v>110.6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.015</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" s="3">
-        <v>128.0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>1.08</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.07</v>
+        <v>112.6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0.025</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" s="3">
-        <v>143.0</v>
-      </c>
-      <c r="B7" s="4">
-        <v>1.61</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.05</v>
+        <v>114.6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0.025</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="3">
-        <v>167.0</v>
-      </c>
-      <c r="B8" s="4">
-        <v>2.2</v>
-      </c>
-      <c r="C8" s="4">
-        <v>0.08</v>
+        <v>120.6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.37</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.02</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
     <row r="9">
-      <c r="A9" s="3">
-        <v>194.0</v>
-      </c>
-      <c r="B9" s="4">
-        <v>2.54</v>
-      </c>
-      <c r="C9" s="4">
-        <v>0.07</v>
+      <c r="A9" s="4">
+        <v>130.5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.74</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.04</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
-      <c r="A10" s="3">
-        <v>240.0</v>
-      </c>
-      <c r="B10" s="4">
-        <v>2.81</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0.04</v>
+      <c r="A10" s="4">
+        <v>140.5</v>
+      </c>
+      <c r="B10" s="3">
+        <v>1.02</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.045</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
-      <c r="A11" s="3">
-        <v>288.0</v>
-      </c>
-      <c r="B11" s="4">
-        <v>2.93</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.03</v>
+      <c r="A11" s="4">
+        <v>150.4</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.15</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.055</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
-      <c r="A12" s="3">
-        <v>338.0</v>
-      </c>
-      <c r="B12" s="4">
-        <v>2.88</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.03</v>
+      <c r="A12" s="4">
+        <v>160.2</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0.055</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
-      <c r="A13" s="3">
-        <v>387.0</v>
-      </c>
-      <c r="B13" s="4">
-        <v>2.87</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.03</v>
+      <c r="A13" s="4">
+        <v>170.2</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="C13" s="3">
+        <v>0.065</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
-      <c r="A14" s="3">
-        <v>485.0</v>
-      </c>
-      <c r="B14" s="4">
-        <v>2.66</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0.02</v>
+      <c r="A14" s="4">
+        <v>180.1</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.44</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.065</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
-      <c r="A15" s="3">
-        <v>520.0</v>
-      </c>
-      <c r="B15" s="4">
-        <v>2.67</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0.03</v>
+      <c r="A15" s="4">
+        <v>200.7</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1.73</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.08</v>
       </c>
       <c r="D15" s="6"/>
     </row>
     <row r="16">
-      <c r="A16" s="3">
-        <v>544.0</v>
-      </c>
-      <c r="B16" s="4">
-        <v>2.6</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0.04</v>
+      <c r="A16" s="4">
+        <v>251.5</v>
+      </c>
+      <c r="B16" s="3">
+        <v>1.87</v>
+      </c>
+      <c r="C16" s="3">
+        <v>0.085</v>
       </c>
       <c r="D16" s="6"/>
     </row>
     <row r="17">
-      <c r="A17" s="3">
-        <v>570.0</v>
-      </c>
-      <c r="B17" s="4">
-        <v>2.67</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0.03</v>
+      <c r="A17" s="4">
+        <v>301.6</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2.03</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.085</v>
       </c>
       <c r="D17" s="6"/>
     </row>
     <row r="18">
-      <c r="A18" s="3">
-        <v>584.0</v>
-      </c>
-      <c r="B18" s="4">
-        <v>2.7</v>
+      <c r="A18" s="4">
+        <v>351.9</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.99</v>
       </c>
       <c r="C18" s="7">
-        <v>0.02</v>
+        <v>0.085</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19">
-      <c r="A19" s="3">
-        <v>604.0</v>
-      </c>
-      <c r="B19" s="4">
-        <v>2.65</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0.03</v>
+      <c r="A19" s="4">
+        <v>402.0</v>
+      </c>
+      <c r="B19" s="3">
+        <v>1.88</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0.08</v>
       </c>
       <c r="D19" s="6"/>
       <c r="F19" s="7"/>
     </row>
     <row r="20">
-      <c r="A20" s="3">
-        <v>634.0</v>
-      </c>
-      <c r="B20" s="3">
-        <v>2.71</v>
-      </c>
-      <c r="C20" s="3">
-        <v>0.03</v>
+      <c r="A20" s="4">
+        <v>452.2</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="C20" s="4">
+        <v>0.08</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="8"/>
       <c r="F20" s="7"/>
     </row>
     <row r="21">
-      <c r="A21" s="3">
-        <v>663.0</v>
-      </c>
-      <c r="B21" s="3">
-        <v>2.6</v>
-      </c>
-      <c r="C21" s="3">
-        <v>0.05</v>
+      <c r="A21" s="4">
+        <v>502.2</v>
+      </c>
+      <c r="B21" s="4">
+        <v>1.79</v>
+      </c>
+      <c r="C21" s="4">
+        <v>0.075</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="8"/>
       <c r="F21" s="7"/>
     </row>
     <row r="22">
-      <c r="A22" s="3">
-        <v>693.0</v>
-      </c>
-      <c r="B22" s="3">
-        <v>2.59</v>
-      </c>
-      <c r="C22" s="3">
-        <v>0.05</v>
+      <c r="A22" s="4">
+        <v>542.3</v>
+      </c>
+      <c r="B22" s="4">
+        <v>1.78</v>
+      </c>
+      <c r="C22" s="4">
+        <v>0.075</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="8"/>
       <c r="F22" s="7"/>
     </row>
     <row r="23">
-      <c r="A23" s="3">
-        <v>783.0</v>
-      </c>
-      <c r="B23" s="3">
-        <v>2.38</v>
-      </c>
-      <c r="C23" s="3">
-        <v>0.02</v>
+      <c r="A23" s="4">
+        <v>552.3</v>
+      </c>
+      <c r="B23" s="4">
+        <v>1.8</v>
+      </c>
+      <c r="C23" s="4">
+        <v>0.075</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="8"/>
       <c r="F23" s="7"/>
     </row>
     <row r="24">
-      <c r="A24" s="3">
-        <v>980.0</v>
-      </c>
-      <c r="B24" s="3">
-        <v>2.04</v>
-      </c>
-      <c r="C24" s="3">
-        <v>0.03</v>
+      <c r="A24" s="4">
+        <v>562.4</v>
+      </c>
+      <c r="B24" s="4">
+        <v>1.81</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0.075</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="8"/>
       <c r="F24" s="7"/>
     </row>
     <row r="25">
-      <c r="A25" s="3">
-        <v>1177.0</v>
-      </c>
-      <c r="B25" s="3">
-        <v>1.87</v>
-      </c>
-      <c r="C25" s="3">
-        <v>0.03</v>
+      <c r="A25" s="4">
+        <v>572.4</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="C25" s="4">
+        <v>0.075</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="8"/>
       <c r="F25" s="7"/>
     </row>
     <row r="26">
-      <c r="A26" s="3">
-        <v>1475.0</v>
-      </c>
-      <c r="B26" s="3">
-        <v>1.46</v>
-      </c>
-      <c r="C26" s="3">
-        <v>0.02</v>
+      <c r="A26" s="4">
+        <v>582.5</v>
+      </c>
+      <c r="B26" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="C26" s="4">
+        <v>0.08</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="8"/>
       <c r="F26" s="7"/>
     </row>
     <row r="27">
-      <c r="A27" s="3"/>
-      <c r="B27" s="3"/>
+      <c r="A27" s="4">
+        <v>592.5</v>
+      </c>
+      <c r="B27" s="4">
+        <v>1.84</v>
+      </c>
+      <c r="C27" s="4">
+        <v>0.08</v>
+      </c>
       <c r="D27" s="9"/>
       <c r="E27" s="8"/>
       <c r="F27" s="7"/>
     </row>
     <row r="28">
+      <c r="A28" s="4">
+        <v>602.5</v>
+      </c>
+      <c r="B28" s="4">
+        <v>1.84</v>
+      </c>
+      <c r="C28" s="4">
+        <v>0.075</v>
+      </c>
       <c r="D28" s="9"/>
       <c r="E28" s="8"/>
       <c r="F28" s="7"/>
     </row>
     <row r="29">
+      <c r="A29" s="4">
+        <v>612.7</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1.82</v>
+      </c>
+      <c r="C29" s="4">
+        <v>0.075</v>
+      </c>
       <c r="D29" s="9"/>
       <c r="E29" s="8"/>
       <c r="F29" s="7"/>
     </row>
     <row r="30">
+      <c r="A30" s="4">
+        <v>622.6</v>
+      </c>
+      <c r="B30" s="4">
+        <v>1.77</v>
+      </c>
+      <c r="C30" s="4">
+        <v>0.075</v>
+      </c>
       <c r="D30" s="9"/>
       <c r="E30" s="8"/>
       <c r="F30" s="7"/>
     </row>
     <row r="31">
+      <c r="A31" s="4">
+        <v>652.7</v>
+      </c>
+      <c r="B31" s="4">
+        <v>1.86</v>
+      </c>
+      <c r="C31" s="4">
+        <v>0.085</v>
+      </c>
       <c r="D31" s="9"/>
       <c r="E31" s="8"/>
       <c r="F31" s="7"/>
     </row>
     <row r="32">
+      <c r="A32" s="4">
+        <v>703.1</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1.76</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.085</v>
+      </c>
       <c r="D32" s="9"/>
       <c r="E32" s="8"/>
       <c r="F32" s="7"/>
     </row>
     <row r="33">
+      <c r="A33" s="4">
+        <v>753.3</v>
+      </c>
+      <c r="B33" s="4">
+        <v>1.69</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.08</v>
+      </c>
       <c r="D33" s="9"/>
       <c r="E33" s="8"/>
       <c r="F33" s="7"/>
     </row>
     <row r="34">
+      <c r="A34" s="4">
+        <v>803.5</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1.66</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.07</v>
+      </c>
       <c r="D34" s="9"/>
       <c r="E34" s="8"/>
       <c r="F34" s="7"/>
     </row>
     <row r="35">
+      <c r="A35" s="4">
+        <v>853.8</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1.54</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.07</v>
+      </c>
       <c r="D35" s="9"/>
       <c r="E35" s="8"/>
     </row>
     <row r="36">
+      <c r="A36" s="4">
+        <v>903.8</v>
+      </c>
+      <c r="B36" s="4">
+        <v>1.55</v>
+      </c>
+      <c r="C36" s="4">
+        <v>0.065</v>
+      </c>
       <c r="D36" s="10"/>
       <c r="E36" s="9"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="4">
+        <v>954.3</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1.56</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.075</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4">
+        <v>1004.7</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1.54</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.065</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4">
+        <v>1204.6</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1.26</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.055</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4">
+        <v>1505.8</v>
+      </c>
+      <c r="B40" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="C40" s="4">
+        <v>0.06</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Finished checks for oxygen uncertainties and reran codes.
</commit_message>
<xml_diff>
--- a/csdata/O/SI/O4+.xlsx
+++ b/csdata/O/SI/O4+.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gmondeel/Documents/CfA/Chandra/CHANDRA-Rates/csdata/O/SI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEE83CE-6961-4941-BA17-984C0F5372AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7440E395-322D-984C-9940-CCD505664345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="760" windowWidth="15140" windowHeight="8740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -361,7 +361,7 @@
   <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F1" sqref="F1:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>